<commit_message>
Updating with more functionalities
</commit_message>
<xml_diff>
--- a/src/vendingMachine/snacks.xlsx
+++ b/src/vendingMachine/snacks.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekty\Python\vending-machine\vendingMachine\src\vendingMachine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F169FA5-003E-479F-82D8-C930D7B66C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CC50B5-9261-4427-A827-57EE531D12CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10500" yWindow="3465" windowWidth="17280" windowHeight="9030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -39,13 +34,13 @@
     <t>Marshmallows</t>
   </si>
   <si>
+    <t>Gummy bears</t>
+  </si>
+  <si>
     <t>Cola</t>
   </si>
   <si>
     <t>Water</t>
-  </si>
-  <si>
-    <t>Gummy bears</t>
   </si>
 </sst>
 </file>
@@ -367,7 +362,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +416,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>6</v>
@@ -432,7 +427,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>2.7</v>
@@ -443,7 +438,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>0.8</v>
@@ -454,6 +449,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>